<commit_message>
La tabla normalizada con los detalles.
</commit_message>
<xml_diff>
--- a/BD/Tabla Normalizada.xlsx
+++ b/BD/Tabla Normalizada.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="104">
   <si>
     <t>Id_alumno</t>
   </si>
@@ -303,6 +303,39 @@
   </si>
   <si>
     <t>Id_alumno FK</t>
+  </si>
+  <si>
+    <t>FK Id_alumno</t>
+  </si>
+  <si>
+    <t>FORMA 1</t>
+  </si>
+  <si>
+    <t>COLONIA</t>
+  </si>
+  <si>
+    <t>NUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lopez mateos </t>
+  </si>
+  <si>
+    <t>ape_docente_pat</t>
+  </si>
+  <si>
+    <t>ape_docente_mat</t>
+  </si>
+  <si>
+    <t>FK Id_materia</t>
+  </si>
+  <si>
+    <t>FK Id_Carrera</t>
+  </si>
+  <si>
+    <t>FORMA 3</t>
+  </si>
+  <si>
+    <t>FK Id_docente</t>
   </si>
 </sst>
 </file>
@@ -505,7 +538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -592,6 +625,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -873,10 +909,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L65"/>
+  <dimension ref="A1:AG100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="P56" sqref="P56"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2:Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,9 +928,16 @@
     <col min="9" max="9" width="12.28515625" customWidth="1"/>
     <col min="10" max="10" width="9.7109375" customWidth="1"/>
     <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="26" max="26" width="10.42578125" customWidth="1"/>
+    <col min="27" max="27" width="13.42578125" customWidth="1"/>
+    <col min="30" max="30" width="16.85546875" customWidth="1"/>
+    <col min="31" max="31" width="16.7109375" customWidth="1"/>
+    <col min="32" max="32" width="9.28515625" customWidth="1"/>
+    <col min="33" max="33" width="13" customWidth="1"/>
+    <col min="34" max="34" width="7.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -928,8 +971,14 @@
       <c r="K1" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N1">
+        <v>1</v>
+      </c>
+      <c r="P1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -963,8 +1012,63 @@
       <c r="K2" s="8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N2">
+        <v>2</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="W2" s="31"/>
+      <c r="X2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16">
         <v>1</v>
       </c>
@@ -998,8 +1102,63 @@
       <c r="K3" s="8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="P3" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="U3" s="9">
+        <v>232</v>
+      </c>
+      <c r="V3" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="W3" s="21"/>
+      <c r="X3" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA3" s="30">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC3" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE3" s="15">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG3" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16">
         <v>1</v>
       </c>
@@ -1033,8 +1192,63 @@
       <c r="K4" s="8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N4">
+        <v>4</v>
+      </c>
+      <c r="P4" s="17">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="S4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="U4" s="9">
+        <v>230</v>
+      </c>
+      <c r="V4" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="W4" s="21"/>
+      <c r="X4" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA4" s="30">
+        <v>2</v>
+      </c>
+      <c r="AB4" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC4" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD4" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE4" s="15">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG4" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
         <v>2</v>
       </c>
@@ -1068,8 +1282,63 @@
       <c r="K5" s="8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N5">
+        <v>5</v>
+      </c>
+      <c r="P5" s="17">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="S5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="T5" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="U5" s="9">
+        <v>1220</v>
+      </c>
+      <c r="V5" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="W5" s="21"/>
+      <c r="X5" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA5" s="30">
+        <v>2</v>
+      </c>
+      <c r="AB5" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC5" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD5" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE5" s="15">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG5" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17">
         <v>2</v>
       </c>
@@ -1101,10 +1370,44 @@
         <v>33</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="N6">
+        <v>6</v>
+      </c>
+      <c r="W6" s="21"/>
+      <c r="X6" s="17">
+        <v>2</v>
+      </c>
+      <c r="Y6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA6" s="30">
+        <v>3</v>
+      </c>
+      <c r="AB6" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC6" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD6" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE6" s="15">
+        <v>2</v>
+      </c>
+      <c r="AF6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG6" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>3</v>
       </c>
@@ -1138,18 +1441,129 @@
       <c r="K7" s="13" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="N7">
+        <v>7</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W7" s="21"/>
+      <c r="X7" s="17">
+        <v>2</v>
+      </c>
+      <c r="Y7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA7" s="30">
+        <v>4</v>
+      </c>
+      <c r="AB7" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC7" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD7" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE7" s="23">
+        <v>2</v>
+      </c>
+      <c r="AF7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG7" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N8">
+        <v>8</v>
+      </c>
+      <c r="P8" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="W8" s="21"/>
+      <c r="X8" s="17">
+        <v>3</v>
+      </c>
+      <c r="Y8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z8" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA8" s="30">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC8" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD8" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE8" s="18">
+        <v>3</v>
+      </c>
+      <c r="AF8" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG8" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N9">
+        <v>9</v>
+      </c>
+      <c r="P9" s="17">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="19" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N10">
+        <v>10</v>
+      </c>
+      <c r="P10" s="17">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N11">
+        <v>11</v>
+      </c>
+      <c r="P11" s="17">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1186,8 +1600,13 @@
       <c r="L12" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N12">
+        <v>12</v>
+      </c>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="21"/>
+    </row>
+    <row r="13" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16">
         <v>1</v>
       </c>
@@ -1222,8 +1641,13 @@
       <c r="L13" s="17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N13">
+        <v>13</v>
+      </c>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="21"/>
+    </row>
+    <row r="14" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
         <v>2</v>
       </c>
@@ -1260,8 +1684,11 @@
       <c r="L14" s="17" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>3</v>
       </c>
@@ -1296,8 +1723,102 @@
       <c r="L15" s="17" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N15">
+        <v>15</v>
+      </c>
+      <c r="P15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N16">
+        <v>16</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC16" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N17">
+        <v>17</v>
+      </c>
+      <c r="P17" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="R17" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="S17" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="T17" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="U17" s="9">
+        <v>232</v>
+      </c>
+      <c r="V17" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="X17" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z17" s="30">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB17" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC17" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -1305,8 +1826,50 @@
         <v>65</v>
       </c>
       <c r="J18" s="22"/>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N18">
+        <v>18</v>
+      </c>
+      <c r="P18" s="17">
+        <v>2</v>
+      </c>
+      <c r="Q18" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R18" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="S18" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="T18" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="U18" s="9">
+        <v>230</v>
+      </c>
+      <c r="V18" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="X18" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z18" s="30">
+        <v>2</v>
+      </c>
+      <c r="AA18" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB18" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC18" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>79</v>
       </c>
@@ -1328,8 +1891,51 @@
       <c r="H19" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N19">
+        <v>19</v>
+      </c>
+      <c r="P19" s="17">
+        <v>3</v>
+      </c>
+      <c r="Q19" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="R19" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="S19" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="T19" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="U19" s="9">
+        <v>1220</v>
+      </c>
+      <c r="V19" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="W19" s="31"/>
+      <c r="X19" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z19" s="30">
+        <v>2</v>
+      </c>
+      <c r="AA19" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB19" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC19" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17">
         <v>1</v>
       </c>
@@ -1351,8 +1957,30 @@
       <c r="H20" s="15" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N20">
+        <v>20</v>
+      </c>
+      <c r="W20" s="21"/>
+      <c r="X20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z20" s="30">
+        <v>3</v>
+      </c>
+      <c r="AA20" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB20" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC20" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="17">
         <v>2</v>
       </c>
@@ -1374,8 +2002,42 @@
       <c r="H21" s="15" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N21">
+        <v>21</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="W21" s="21"/>
+      <c r="X21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y21" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z21" s="30">
+        <v>4</v>
+      </c>
+      <c r="AA21" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB21" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC21" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17">
         <v>2</v>
       </c>
@@ -1397,8 +2059,24 @@
       <c r="H22" s="15" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N22">
+        <v>22</v>
+      </c>
+      <c r="P22" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="S22" s="17">
+        <v>1</v>
+      </c>
+      <c r="T22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="W22" s="21"/>
+    </row>
+    <row r="23" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="17">
         <v>3</v>
       </c>
@@ -1420,8 +2098,24 @@
       <c r="H23" s="23" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N23">
+        <v>23</v>
+      </c>
+      <c r="P23" s="17">
+        <v>2</v>
+      </c>
+      <c r="Q23" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="S23" s="17">
+        <v>1</v>
+      </c>
+      <c r="T23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="W23" s="21"/>
+    </row>
+    <row r="24" spans="1:29" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="17">
         <v>4</v>
       </c>
@@ -1431,23 +2125,144 @@
       <c r="C24" s="9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="N24">
+        <v>24</v>
+      </c>
+      <c r="P24" s="17">
+        <v>2</v>
+      </c>
+      <c r="Q24" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="S24" s="17">
+        <v>1</v>
+      </c>
+      <c r="T24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="W24" s="21"/>
+      <c r="X24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC24" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="20"/>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
-    </row>
-    <row r="27" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="N25">
+        <v>25</v>
+      </c>
+      <c r="P25" s="17">
+        <v>3</v>
+      </c>
+      <c r="Q25" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="S25" s="17">
+        <v>2</v>
+      </c>
+      <c r="T25" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="W25" s="21"/>
+      <c r="X25" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z25" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB25" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC25" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N26">
+        <v>26</v>
+      </c>
+      <c r="S26" s="17">
+        <v>2</v>
+      </c>
+      <c r="T26" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="X26" s="17">
+        <v>2</v>
+      </c>
+      <c r="Y26" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z26" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB26" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC26" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="29" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N27">
+        <v>27</v>
+      </c>
+      <c r="S27" s="17">
+        <v>3</v>
+      </c>
+      <c r="T27" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="X27" s="17">
+        <v>3</v>
+      </c>
+      <c r="Y27" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z27" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB27" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC27" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N28">
+        <v>28</v>
+      </c>
+      <c r="AB28" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC28" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>83</v>
       </c>
@@ -1478,8 +2293,17 @@
       <c r="J29" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N29">
+        <v>29</v>
+      </c>
+      <c r="AB29" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC29" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17">
         <v>1</v>
       </c>
@@ -1508,8 +2332,17 @@
       <c r="J30" s="9" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N30">
+        <v>30</v>
+      </c>
+      <c r="AB30" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC30" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17">
         <v>2</v>
       </c>
@@ -1540,8 +2373,11 @@
       <c r="J31" s="9" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N31">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17">
         <v>3</v>
       </c>
@@ -1570,8 +2406,16 @@
       <c r="J32" s="9" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N32">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="N33">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -1581,8 +2425,14 @@
       <c r="J34" s="22" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N34">
+        <v>34</v>
+      </c>
+      <c r="P34" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>79</v>
       </c>
@@ -1613,8 +2463,32 @@
       <c r="L35" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N35">
+        <v>35</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="V35" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17">
         <v>1</v>
       </c>
@@ -1645,8 +2519,32 @@
       <c r="L36" s="17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N36">
+        <v>36</v>
+      </c>
+      <c r="P36" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="R36" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="S36" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="T36" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="U36" s="9">
+        <v>232</v>
+      </c>
+      <c r="V36" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="17">
         <v>2</v>
       </c>
@@ -1677,8 +2575,32 @@
       <c r="L37" s="17" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N37">
+        <v>37</v>
+      </c>
+      <c r="P37" s="17">
+        <v>2</v>
+      </c>
+      <c r="Q37" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R37" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="S37" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="T37" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="U37" s="9">
+        <v>230</v>
+      </c>
+      <c r="V37" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="17">
         <v>2</v>
       </c>
@@ -1709,8 +2631,42 @@
       <c r="L38" s="17" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N38">
+        <v>38</v>
+      </c>
+      <c r="P38" s="17">
+        <v>3</v>
+      </c>
+      <c r="Q38" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="R38" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="S38" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="T38" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="U38" s="9">
+        <v>1220</v>
+      </c>
+      <c r="V38" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="W38" s="31"/>
+      <c r="X38" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z38" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="17">
         <v>3</v>
       </c>
@@ -1732,8 +2688,21 @@
       <c r="H39" s="23" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N39">
+        <v>39</v>
+      </c>
+      <c r="W39" s="21"/>
+      <c r="X39" s="30">
+        <v>1</v>
+      </c>
+      <c r="Y39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z39" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="17">
         <v>4</v>
       </c>
@@ -1743,18 +2712,138 @@
       <c r="C40" s="9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="N40">
+        <v>40</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q40" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S40" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="T40" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="W40" s="21"/>
+      <c r="X40" s="30">
+        <v>2</v>
+      </c>
+      <c r="Y40" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z40" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N41">
+        <v>41</v>
+      </c>
+      <c r="P41" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="S41" s="17">
+        <v>1</v>
+      </c>
+      <c r="T41" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="W41" s="21"/>
+      <c r="X41" s="30">
+        <v>2</v>
+      </c>
+      <c r="Y41" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z41" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N42">
+        <v>42</v>
+      </c>
+      <c r="P42" s="17">
+        <v>2</v>
+      </c>
+      <c r="Q42" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="S42" s="17">
+        <v>1</v>
+      </c>
+      <c r="T42" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="W42" s="21"/>
+      <c r="X42" s="30">
+        <v>3</v>
+      </c>
+      <c r="Y42" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z42" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="29" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N43">
+        <v>43</v>
+      </c>
+      <c r="P43" s="17">
+        <v>2</v>
+      </c>
+      <c r="Q43" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="S43" s="17">
+        <v>1</v>
+      </c>
+      <c r="T43" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="W43" s="21"/>
+      <c r="X43" s="30">
+        <v>4</v>
+      </c>
+      <c r="Y43" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z43" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N44">
+        <v>44</v>
+      </c>
+      <c r="P44" s="17">
+        <v>3</v>
+      </c>
+      <c r="Q44" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="S44" s="17">
+        <v>2</v>
+      </c>
+      <c r="T44" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="W44" s="21"/>
+    </row>
+    <row r="45" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>83</v>
       </c>
@@ -1785,8 +2874,17 @@
       <c r="J45" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N45">
+        <v>45</v>
+      </c>
+      <c r="S45" s="17">
+        <v>2</v>
+      </c>
+      <c r="T45" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="17">
         <v>1</v>
       </c>
@@ -1815,8 +2913,17 @@
       <c r="J46" s="9" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N46">
+        <v>46</v>
+      </c>
+      <c r="S46" s="17">
+        <v>3</v>
+      </c>
+      <c r="T46" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="17">
         <v>2</v>
       </c>
@@ -1847,8 +2954,23 @@
       <c r="J47" s="9" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N47">
+        <v>47</v>
+      </c>
+      <c r="W47" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="X47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y47" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z47" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="17">
         <v>3</v>
       </c>
@@ -1877,16 +2999,108 @@
       <c r="J48" s="9" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N48">
+        <v>48</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q48" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R48" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T48" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="U48" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="W48" s="30">
+        <v>1</v>
+      </c>
+      <c r="X48" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y48" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z48" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N49">
+        <v>49</v>
+      </c>
+      <c r="P49" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q49" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="R49" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="T49" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="U49" s="15">
+        <v>1</v>
+      </c>
+      <c r="W49" s="30">
+        <v>2</v>
+      </c>
+      <c r="X49" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y49" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z49" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:26" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>64</v>
       </c>
       <c r="E50" s="22" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N50">
+        <v>50</v>
+      </c>
+      <c r="P50" s="17">
+        <v>2</v>
+      </c>
+      <c r="Q50" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="R50" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="T50" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="U50" s="15">
+        <v>1</v>
+      </c>
+      <c r="W50" s="30">
+        <v>3</v>
+      </c>
+      <c r="X50" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y50" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z50" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>79</v>
       </c>
@@ -1908,8 +3122,38 @@
       <c r="H51" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N51">
+        <v>51</v>
+      </c>
+      <c r="P51" s="17">
+        <v>3</v>
+      </c>
+      <c r="Q51" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="R51" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="T51" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="U51" s="15">
+        <v>1</v>
+      </c>
+      <c r="W51" s="30">
+        <v>4</v>
+      </c>
+      <c r="X51" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y51" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z51" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="17">
         <v>1</v>
       </c>
@@ -1931,8 +3175,17 @@
       <c r="H52" s="15" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N52">
+        <v>52</v>
+      </c>
+      <c r="T52" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="U52" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="17">
         <v>2</v>
       </c>
@@ -1954,8 +3207,17 @@
       <c r="H53" s="15" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N53">
+        <v>53</v>
+      </c>
+      <c r="T53" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="U53" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="17">
         <v>2</v>
       </c>
@@ -1977,8 +3239,17 @@
       <c r="H54" s="15" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N54">
+        <v>54</v>
+      </c>
+      <c r="T54" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="U54" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="17">
         <v>3</v>
       </c>
@@ -2000,8 +3271,11 @@
       <c r="H55" s="23" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N55">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="17">
         <v>4</v>
       </c>
@@ -2011,16 +3285,27 @@
       <c r="C56" s="9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N56">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="N57">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>78</v>
       </c>
       <c r="D58" s="22" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N58">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>91</v>
       </c>
@@ -2036,8 +3321,11 @@
       <c r="F59" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N59">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
         <v>9</v>
       </c>
@@ -2053,8 +3341,11 @@
       <c r="F60" s="17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N60">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
         <v>12</v>
       </c>
@@ -2070,8 +3361,11 @@
       <c r="F61" s="17" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N61">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
         <v>15</v>
       </c>
@@ -2087,29 +3381,216 @@
       <c r="F62" s="17" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N62">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B63" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N63">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B64" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N64">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B65" s="17">
         <v>3</v>
+      </c>
+      <c r="N65">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N66">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N67">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N68">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N69">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N70">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N71">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N72">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N73">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N74">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N75">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N76">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N77">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N78">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N79">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N80">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N81">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N82">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="83" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N83">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N84">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N85">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N86">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N87">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N88">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N89">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N90">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N91">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="92" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N92">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N93">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N94">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N95">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="96" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N96">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N97">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="98" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N98">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="99" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N99">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N100">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2119,15 +3600,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010073E838899453484ABFEEAF127705302F" ma:contentTypeVersion="5" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="cdeacefbf8b7e139c1e3154d83511088">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6a30442a-90f0-46be-8c2f-570cb496af53" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9fcb6e85bb80f3d4c793162617e10913" ns2:_="">
     <xsd:import namespace="6a30442a-90f0-46be-8c2f-570cb496af53"/>
@@ -2277,15 +3749,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AA610A8-0906-428A-95F9-BFC2E55B36A1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEAB7907-1C8E-4E3C-979E-FC22FB1ECBF6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2301,4 +3774,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AA610A8-0906-428A-95F9-BFC2E55B36A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
La tabla normalizada con los detalles y el documento perron.
</commit_message>
<xml_diff>
--- a/BD/Tabla Normalizada.xlsx
+++ b/BD/Tabla Normalizada.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="108">
   <si>
     <t>Id_alumno</t>
   </si>
@@ -336,6 +336,18 @@
   </si>
   <si>
     <t>FK Id_docente</t>
+  </si>
+  <si>
+    <t>Alumno</t>
+  </si>
+  <si>
+    <t>Alumno_Telefono</t>
+  </si>
+  <si>
+    <t>Alumno_Materia</t>
+  </si>
+  <si>
+    <t>Materia</t>
   </si>
 </sst>
 </file>
@@ -538,7 +550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -628,6 +640,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -909,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG100"/>
+  <dimension ref="A1:AG111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2:Y8"/>
+    <sheetView tabSelected="1" topLeftCell="N51" zoomScale="95" workbookViewId="0">
+      <selection activeCell="AC39" sqref="AC39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,6 +961,7 @@
     <col min="9" max="9" width="12.28515625" customWidth="1"/>
     <col min="10" max="10" width="9.7109375" customWidth="1"/>
     <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" customWidth="1"/>
     <col min="26" max="26" width="10.42578125" customWidth="1"/>
     <col min="27" max="27" width="13.42578125" customWidth="1"/>
     <col min="30" max="30" width="16.85546875" customWidth="1"/>
@@ -1027,13 +1061,13 @@
       <c r="S2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="T2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="U2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="V2" s="1" t="s">
         <v>95</v>
       </c>
       <c r="W2" s="31"/>
@@ -1117,7 +1151,7 @@
       <c r="S3" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="T3" s="5" t="s">
+      <c r="T3" s="9" t="s">
         <v>97</v>
       </c>
       <c r="U3" s="9">
@@ -1207,7 +1241,7 @@
       <c r="S4" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="T4" s="5" t="s">
+      <c r="T4" s="9" t="s">
         <v>58</v>
       </c>
       <c r="U4" s="9">
@@ -1297,7 +1331,7 @@
       <c r="S5" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="T5" s="13" t="s">
+      <c r="T5" s="9" t="s">
         <v>59</v>
       </c>
       <c r="U5" s="9">
@@ -2410,12 +2444,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="N33">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -2432,7 +2466,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>79</v>
       </c>
@@ -2488,7 +2522,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17">
         <v>1</v>
       </c>
@@ -2544,7 +2578,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="17">
         <v>2</v>
       </c>
@@ -2600,7 +2634,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="1:26" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:27" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="17">
         <v>2</v>
       </c>
@@ -2666,7 +2700,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:26" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:27" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="17">
         <v>3</v>
       </c>
@@ -2702,7 +2736,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:26" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:27" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="17">
         <v>4</v>
       </c>
@@ -2738,7 +2772,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N41">
         <v>41</v>
       </c>
@@ -2765,7 +2799,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:26" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:27" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N42">
         <v>42</v>
       </c>
@@ -2792,7 +2826,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:26" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:27" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="29" t="s">
         <v>87</v>
       </c>
@@ -2822,7 +2856,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>63</v>
       </c>
@@ -2843,7 +2877,7 @@
       </c>
       <c r="W44" s="21"/>
     </row>
-    <row r="45" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:27" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>83</v>
       </c>
@@ -2883,8 +2917,20 @@
       <c r="T45" s="9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="46" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z45" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA45" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="17">
         <v>1</v>
       </c>
@@ -2922,8 +2968,20 @@
       <c r="T46" s="13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="47" spans="1:26" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X46" s="30">
+        <v>1</v>
+      </c>
+      <c r="Y46" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z46" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA46" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="17">
         <v>2</v>
       </c>
@@ -2957,20 +3015,20 @@
       <c r="N47">
         <v>47</v>
       </c>
-      <c r="W47" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="X47" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y47" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z47" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="48" spans="1:26" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X47" s="30">
+        <v>2</v>
+      </c>
+      <c r="Y47" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z47" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA47" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="17">
         <v>3</v>
       </c>
@@ -3017,20 +3075,20 @@
       <c r="U48" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="W48" s="30">
-        <v>1</v>
-      </c>
-      <c r="X48" s="8" t="s">
-        <v>74</v>
+      <c r="X48" s="30">
+        <v>3</v>
       </c>
       <c r="Y48" s="8" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="Z48" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="49" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="AA48" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N49">
         <v>49</v>
       </c>
@@ -3049,20 +3107,20 @@
       <c r="U49" s="15">
         <v>1</v>
       </c>
-      <c r="W49" s="30">
-        <v>2</v>
-      </c>
-      <c r="X49" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y49" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z49" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="50" spans="1:26" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X49" s="30">
+        <v>4</v>
+      </c>
+      <c r="Y49" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z49" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA49" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>64</v>
       </c>
@@ -3087,20 +3145,8 @@
       <c r="U50" s="15">
         <v>1</v>
       </c>
-      <c r="W50" s="30">
-        <v>3</v>
-      </c>
-      <c r="X50" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y50" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z50" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="51" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>79</v>
       </c>
@@ -3140,20 +3186,8 @@
       <c r="U51" s="15">
         <v>1</v>
       </c>
-      <c r="W51" s="30">
-        <v>4</v>
-      </c>
-      <c r="X51" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y51" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z51" s="10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="52" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="17">
         <v>1</v>
       </c>
@@ -3185,7 +3219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="17">
         <v>2</v>
       </c>
@@ -3217,7 +3251,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="17">
         <v>2</v>
       </c>
@@ -3249,7 +3283,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="17">
         <v>3</v>
       </c>
@@ -3275,7 +3309,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="17">
         <v>4</v>
       </c>
@@ -3289,12 +3323,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="N57">
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>78</v>
       </c>
@@ -3305,7 +3339,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>91</v>
       </c>
@@ -3325,7 +3359,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
         <v>9</v>
       </c>
@@ -3345,7 +3379,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
         <v>12</v>
       </c>
@@ -3365,7 +3399,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
         <v>15</v>
       </c>
@@ -3385,7 +3419,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
         <v>19</v>
       </c>
@@ -3396,7 +3430,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="9" t="s">
         <v>22</v>
       </c>
@@ -3533,64 +3567,389 @@
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N89">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="90" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N90">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="91" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N91">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="92" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N92">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="93" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N93">
+    <row r="98" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B98" t="s">
+        <v>104</v>
+      </c>
+      <c r="J98" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="99" spans="2:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J99" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K99" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L99" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M99" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N99" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O99" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="P99" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q99" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R99" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="100" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B100" s="17">
+        <v>1</v>
+      </c>
+      <c r="C100" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D100" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E100" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F100" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="G100" s="9">
+        <v>232</v>
+      </c>
+      <c r="H100" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="J100" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K100" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L100" s="30">
+        <v>1</v>
+      </c>
+      <c r="M100" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="N100" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="O100" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="P100" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q100" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R100" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="101" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B101" s="17">
+        <v>2</v>
+      </c>
+      <c r="C101" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D101" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F101" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G101" s="9">
+        <v>230</v>
+      </c>
+      <c r="H101" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="J101" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K101" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L101" s="30">
+        <v>2</v>
+      </c>
+      <c r="M101" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="N101" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="O101" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="P101" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q101" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R101" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="102" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B102" s="17">
+        <v>3</v>
+      </c>
+      <c r="C102" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D102" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E102" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F102" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G102" s="9">
+        <v>1220</v>
+      </c>
+      <c r="H102" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="J102" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K102" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L102" s="30">
+        <v>2</v>
+      </c>
+      <c r="M102" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="N102" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="O102" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="P102" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q102" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R102" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="103" spans="2:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J103" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K103" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L103" s="30">
+        <v>3</v>
+      </c>
+      <c r="M103" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="N103" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O103" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="P103" s="15">
+        <v>2</v>
+      </c>
+      <c r="Q103" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="R103" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="104" spans="2:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B104" t="s">
+        <v>105</v>
+      </c>
+      <c r="E104" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="J104" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K104" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L104" s="30">
+        <v>4</v>
+      </c>
+      <c r="M104" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="N104" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="O104" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="P104" s="23">
+        <v>2</v>
+      </c>
+      <c r="Q104" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="R104" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="105" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B105" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="94" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N94">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="95" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N95">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="96" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N96">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="97" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N97">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="98" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N98">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="99" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N99">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="100" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N100">
+      <c r="C105" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E105" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="F105" s="33" t="s">
         <v>100</v>
+      </c>
+      <c r="J105" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K105" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L105" s="30">
+        <v>1</v>
+      </c>
+      <c r="M105" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="N105" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="O105" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="P105" s="18">
+        <v>3</v>
+      </c>
+      <c r="Q105" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="R105" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="106" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B106" s="17">
+        <v>1</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E106" s="37">
+        <v>1</v>
+      </c>
+      <c r="F106" s="34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B107" s="17">
+        <v>2</v>
+      </c>
+      <c r="C107" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E107" s="37">
+        <v>1</v>
+      </c>
+      <c r="F107" s="34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="108" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B108" s="17">
+        <v>2</v>
+      </c>
+      <c r="C108" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E108" s="37">
+        <v>1</v>
+      </c>
+      <c r="F108" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="109" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B109" s="17">
+        <v>3</v>
+      </c>
+      <c r="C109" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E109" s="37">
+        <v>2</v>
+      </c>
+      <c r="F109" s="34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="110" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E110" s="37">
+        <v>2</v>
+      </c>
+      <c r="F110" s="35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="111" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E111" s="37">
+        <v>3</v>
+      </c>
+      <c r="F111" s="36" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -3600,6 +3959,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010073E838899453484ABFEEAF127705302F" ma:contentTypeVersion="5" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="cdeacefbf8b7e139c1e3154d83511088">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6a30442a-90f0-46be-8c2f-570cb496af53" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9fcb6e85bb80f3d4c793162617e10913" ns2:_="">
     <xsd:import namespace="6a30442a-90f0-46be-8c2f-570cb496af53"/>
@@ -3749,16 +4117,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AA610A8-0906-428A-95F9-BFC2E55B36A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEAB7907-1C8E-4E3C-979E-FC22FB1ECBF6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3774,12 +4141,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AA610A8-0906-428A-95F9-BFC2E55B36A1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Actualizamos datos de la BD, nuevas clases de Netbeans y un nuevo trabajo de packetaxo
</commit_message>
<xml_diff>
--- a/BD/Tabla Normalizada.xlsx
+++ b/BD/Tabla Normalizada.xlsx
@@ -410,12 +410,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="11">
@@ -550,7 +568,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -661,6 +679,30 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -944,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N51" zoomScale="95" workbookViewId="0">
-      <selection activeCell="AC39" sqref="AC39"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="95" workbookViewId="0">
+      <selection activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,56 +1091,56 @@
       <c r="N2">
         <v>2</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="R2" s="1" t="s">
+      <c r="Q2" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="S2" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="T2" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="U2" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="V2" s="39" t="s">
         <v>95</v>
       </c>
       <c r="W2" s="31"/>
-      <c r="X2" s="1" t="s">
+      <c r="X2" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="Y2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Y2" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z2" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AA2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AB2" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AC2" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AD2" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AE2" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AF2" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AG2" s="40" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1478,10 +1520,10 @@
       <c r="N7">
         <v>7</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="Q7" s="40" t="s">
         <v>2</v>
       </c>
       <c r="W7" s="21"/>
@@ -1768,43 +1810,43 @@
       <c r="N16">
         <v>16</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="P16" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="Q16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="R16" s="1" t="s">
+      <c r="Q16" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="R16" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="S16" s="1" t="s">
+      <c r="S16" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="T16" s="1" t="s">
+      <c r="T16" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="U16" s="1" t="s">
+      <c r="U16" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="V16" s="1" t="s">
+      <c r="V16" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="X16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y16" s="3" t="s">
+      <c r="X16" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y16" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="Z16" s="1" t="s">
+      <c r="Z16" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="AA16" s="2" t="s">
+      <c r="AA16" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="AB16" s="2" t="s">
+      <c r="AB16" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="AC16" s="2" t="s">
+      <c r="AC16" s="43" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2039,16 +2081,16 @@
       <c r="N21">
         <v>21</v>
       </c>
-      <c r="P21" s="1" t="s">
+      <c r="P21" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="Q21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="S21" s="1" t="s">
+      <c r="Q21" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="S21" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="T21" s="2" t="s">
+      <c r="T21" s="43" t="s">
         <v>100</v>
       </c>
       <c r="W21" s="21"/>
@@ -2175,19 +2217,19 @@
         <v>15</v>
       </c>
       <c r="W24" s="21"/>
-      <c r="X24" s="1" t="s">
+      <c r="X24" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="Y24" s="1" t="s">
+      <c r="Y24" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="Z24" s="1" t="s">
+      <c r="Z24" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="AB24" s="1" t="s">
+      <c r="AB24" s="42" t="s">
         <v>100</v>
       </c>
-      <c r="AC24" s="2" t="s">
+      <c r="AC24" s="43" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2500,25 +2542,25 @@
       <c r="N35">
         <v>35</v>
       </c>
-      <c r="P35" s="1" t="s">
+      <c r="P35" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="Q35" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="R35" s="1" t="s">
+      <c r="Q35" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="R35" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="S35" s="1" t="s">
+      <c r="S35" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="T35" s="1" t="s">
+      <c r="T35" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="U35" s="1" t="s">
+      <c r="U35" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="V35" s="1" t="s">
+      <c r="V35" s="45" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2690,13 +2732,13 @@
         <v>60</v>
       </c>
       <c r="W38" s="31"/>
-      <c r="X38" s="1" t="s">
+      <c r="X38" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="Y38" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z38" s="1" t="s">
+      <c r="Y38" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z38" s="45" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2749,16 +2791,16 @@
       <c r="N40">
         <v>40</v>
       </c>
-      <c r="P40" s="1" t="s">
+      <c r="P40" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="Q40" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="S40" s="1" t="s">
+      <c r="Q40" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="S40" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="T40" s="2" t="s">
+      <c r="T40" s="46" t="s">
         <v>100</v>
       </c>
       <c r="W40" s="21"/>
@@ -2917,16 +2959,16 @@
       <c r="T45" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="X45" s="1" t="s">
+      <c r="X45" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="Y45" s="2" t="s">
+      <c r="Y45" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="Z45" s="2" t="s">
+      <c r="Z45" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="AA45" s="2" t="s">
+      <c r="AA45" s="46" t="s">
         <v>99</v>
       </c>
     </row>
@@ -3060,19 +3102,19 @@
       <c r="N48">
         <v>48</v>
       </c>
-      <c r="P48" s="1" t="s">
+      <c r="P48" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="Q48" s="1" t="s">
+      <c r="Q48" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="R48" s="1" t="s">
+      <c r="R48" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="T48" s="1" t="s">
+      <c r="T48" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="U48" s="2" t="s">
+      <c r="U48" s="46" t="s">
         <v>101</v>
       </c>
       <c r="X48" s="30">
@@ -3775,7 +3817,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="103" spans="2:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J103" s="5" t="s">
         <v>19</v>
       </c>
@@ -3959,15 +4001,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010073E838899453484ABFEEAF127705302F" ma:contentTypeVersion="5" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="cdeacefbf8b7e139c1e3154d83511088">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6a30442a-90f0-46be-8c2f-570cb496af53" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9fcb6e85bb80f3d4c793162617e10913" ns2:_="">
     <xsd:import namespace="6a30442a-90f0-46be-8c2f-570cb496af53"/>
@@ -4117,15 +4150,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AA610A8-0906-428A-95F9-BFC2E55B36A1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEAB7907-1C8E-4E3C-979E-FC22FB1ECBF6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4141,4 +4175,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AA610A8-0906-428A-95F9-BFC2E55B36A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>